<commit_message>
reads in updated google cloud files with standardized reaches and updaets metadata accordingly. validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/battle_escapement_raw_metadata.xlsx
+++ b/data-raw/metadata/battle_escapement_raw_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-battle-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1A053F-ACD6-4247-89EC-098911D3B3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D1B21B-ECC7-1A46-A00C-967619E39416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>escapement_raw</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>Method by which the data were collected. Levels = c("video")</t>
   </si>
 </sst>
 </file>
@@ -469,7 +475,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -794,11 +800,21 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="4"/>
+      <c r="A8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>

</xml_diff>